<commit_message>
Se corrigierón detalles menores en ambos documentos
</commit_message>
<xml_diff>
--- a/Organización/Capacitacion/Evaluaciónes/EC_Requerimiento_Ejecución_100715.xlsx
+++ b/Organización/Capacitacion/Evaluaciónes/EC_Requerimiento_Ejecución_100715.xlsx
@@ -81,9 +81,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -303,8 +300,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -312,26 +327,8 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -616,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,23 +623,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" ht="123.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -682,7 +679,7 @@
       <c r="D3" s="13">
         <v>5</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="15">
         <v>5</v>
       </c>
       <c r="F3" s="13">
@@ -697,7 +694,7 @@
       <c r="I3" s="13">
         <v>5</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="17">
         <f>(B3+C3+D3+E3+F3+G3+H3+I3)/8</f>
         <v>4.875</v>
       </c>
@@ -709,12 +706,12 @@
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
-      <c r="E4" s="19"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
-      <c r="J4" s="12"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -744,7 +741,7 @@
       <c r="I5" s="13">
         <v>5</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="17">
         <f t="shared" ref="J5" si="0">(B5+C5+D5+E5+F5+G5+H5+I5)/8</f>
         <v>4.875</v>
       </c>
@@ -761,7 +758,7 @@
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
-      <c r="J6" s="12"/>
+      <c r="J6" s="18"/>
     </row>
     <row r="7" spans="1:10" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -775,7 +772,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
-      <c r="J7" s="11">
+      <c r="J7" s="17">
         <f t="shared" ref="J7" si="1">(B7+C7+D7+E7+F7+G7+H7+I7)/8</f>
         <v>0</v>
       </c>
@@ -792,7 +789,7 @@
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
-      <c r="J8" s="12"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:10" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -806,7 +803,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
-      <c r="J9" s="11">
+      <c r="J9" s="17">
         <f t="shared" ref="J9" si="2">(B9+C9+D9+E9+F9+G9+H9+I9)/8</f>
         <v>0</v>
       </c>
@@ -823,7 +820,7 @@
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
-      <c r="J10" s="12"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" spans="1:10" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -837,7 +834,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
-      <c r="J11" s="11">
+      <c r="J11" s="17">
         <f t="shared" ref="J11" si="3">(B11+C11+D11+E11+F11+G11+H11+I11)/8</f>
         <v>0</v>
       </c>
@@ -854,7 +851,7 @@
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
-      <c r="J12" s="12"/>
+      <c r="J12" s="18"/>
     </row>
     <row r="13" spans="1:10" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -868,7 +865,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
-      <c r="J13" s="11">
+      <c r="J13" s="17">
         <f t="shared" ref="J13" si="4">(B13+C13+D13+E13+F13+G13+H13+I13)/8</f>
         <v>0</v>
       </c>
@@ -885,7 +882,7 @@
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
-      <c r="J14" s="12"/>
+      <c r="J14" s="18"/>
     </row>
     <row r="15" spans="1:10" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -899,7 +896,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
-      <c r="J15" s="11">
+      <c r="J15" s="17">
         <f t="shared" ref="J15" si="5">(B15+C15+D15+E15+F15+G15+H15+I15)/8</f>
         <v>0</v>
       </c>
@@ -916,7 +913,7 @@
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
-      <c r="J16" s="12"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:10" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -930,7 +927,7 @@
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
-      <c r="J17" s="11">
+      <c r="J17" s="17">
         <f t="shared" ref="J17" si="6">(B17+C17+D17+E17+F17+G17+H17+I17)/8</f>
         <v>0</v>
       </c>
@@ -947,7 +944,7 @@
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
-      <c r="J18" s="12"/>
+      <c r="J18" s="18"/>
     </row>
     <row r="19" spans="1:10" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -961,7 +958,7 @@
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
-      <c r="J19" s="11">
+      <c r="J19" s="17">
         <f t="shared" ref="J19" si="7">(B19+C19+D19+E19+F19+G19+H19+I19)/8</f>
         <v>0</v>
       </c>
@@ -978,7 +975,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
-      <c r="J20" s="12"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -992,7 +989,7 @@
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
-      <c r="J21" s="11">
+      <c r="J21" s="17">
         <f t="shared" ref="J21" si="8">(B21+C21+D21+E21+F21+G21+H21+I21)/8</f>
         <v>0</v>
       </c>
@@ -1009,7 +1006,7 @@
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
-      <c r="J22" s="12"/>
+      <c r="J22" s="18"/>
     </row>
     <row r="23" spans="1:10" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
@@ -1023,7 +1020,7 @@
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
-      <c r="J23" s="11">
+      <c r="J23" s="17">
         <f>(B23+C23+D23+E23+F23+G23+H23+I23)/8</f>
         <v>0</v>
       </c>
@@ -1040,7 +1037,7 @@
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
-      <c r="J24" s="12"/>
+      <c r="J24" s="18"/>
     </row>
     <row r="25" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
@@ -1054,34 +1051,76 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="10">
-        <f>(SUM(J3:J6)/2)/5</f>
-        <v>0.97499999999999998</v>
+      <c r="J25" s="19">
+        <f>(SUM(J3:J6)/2)</f>
+        <v>4.875</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="102">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
@@ -1100,69 +1139,27 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>